<commit_message>
[sipedy-15] - Criação backend fornecedores finalizado
</commit_message>
<xml_diff>
--- a/Sistema Sipedy/Especificações Sistema de pedidos.xlsx
+++ b/Sistema Sipedy/Especificações Sistema de pedidos.xlsx
@@ -3,10 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Folha1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr/>
 </workbook>
@@ -189,7 +190,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3">
     <font>
       <name val="Calibri"/>
@@ -266,7 +267,7 @@
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="0" fillId="4" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -278,9 +279,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -796,7 +794,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1019,7 +1017,7 @@
       <c r="B10" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>55</v>
       </c>
       <c r="D10" s="5"/>
@@ -1150,4 +1148,23 @@
   <pageSetup paperSize="9" scale="100" firstPageNumber="2147483647" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="142.140625"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>